<commit_message>
quick data cleaning; added missing negatives
</commit_message>
<xml_diff>
--- a/Finance_Data/2018/Sept_2018.xlsx
+++ b/Finance_Data/2018/Sept_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\Finance_Analysis_PowerBI\Finance_Data\2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4111194-AB91-4D1B-B7D0-416567BF07D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485D969-9972-4629-AED3-B2AE701F215F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-660" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14880" yWindow="870" windowWidth="13575" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>DATE</t>
   </si>
@@ -86,12 +86,6 @@
   </si>
   <si>
     <t>Bake Chef</t>
-  </si>
-  <si>
-    <t>RBC</t>
-  </si>
-  <si>
-    <t>Deposit</t>
   </si>
   <si>
     <t>Dominos</t>
@@ -469,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,79 +726,65 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D18" s="3">
-        <v>158.99</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>43364</v>
+        <v>43368</v>
       </c>
       <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
       <c r="D19" s="3">
-        <v>-33</v>
+        <v>-42.26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>43368</v>
+        <v>43369</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D20" s="3">
-        <v>-42.26</v>
+        <v>-46.22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>43369</v>
+        <v>43371</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3">
-        <v>-46.22</v>
+        <v>-9.1999999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>43371</v>
+        <v>43372</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D22" s="3">
-        <v>-9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>43372</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3">
         <v>-14.37</v>
       </c>
     </row>

</xml_diff>